<commit_message>
Regeneration of files after converter and dictionary update.
</commit_message>
<xml_diff>
--- a/src/main/resources/Слоўнік Пугачова.xlsx
+++ b/src/main/resources/Слоўнік Пугачова.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t xml:space="preserve">BFD</t>
   </si>
@@ -56,6 +56,51 @@
   </si>
   <si>
     <t xml:space="preserve">дыяпазон лікаў для значэньня, якое апісвае вызначаны аспект дызайну канкрэтнага элемента.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CJK Symbols and Punctuation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CJK сымбалі й пунктуацыя</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unicode-блок, які зьмяшчае сымбалі й знакі прыпынку для Кітайскай, Японскай і Карэйскай моў (Chinese, Japanese and Korean)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mkmk, Mark to Mark Positioning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Пазіцыяванне акцэнтаў адносна акцэнтаў</t>
+  </si>
+  <si>
+    <t xml:space="preserve">асаблівасьць OpenType, якая дазваляе пазіцыянаваць акцэнты адносна іншых акцэнтаў</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reverse engineering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Зваротны інжынірынг</t>
+  </si>
+  <si>
+    <t xml:space="preserve">працэс аналізу сістэмы з мэтай зразумець, як яна працуе. Для фізічных аб'ектаў можа ўключаць іх разборку.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Object-oriented programming, OOP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Аб'ектна-арыентаванае праграміраваньне</t>
+  </si>
+  <si>
+    <t xml:space="preserve">падыход да напісаньня коду, пры якім сістэма апісваецца праз аб'екты і іх узаемадзеяньне. Метады й палі з інфармацыяй у гэтым выпадку ня могуць існаваць па-за аб'ектам.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Software design pattern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Шаблёны праграміраваньня, паттэрны праграміраваньня</t>
+  </si>
+  <si>
+    <t xml:space="preserve">агульныя падыходы для рашэньня часта сустракаемых задач, якія могуць выкарыстоўвацца ў розных сістэмах. Не зьяўляюцца канкрэтнымі прыкладамі коду, а апісваюць алгарытм рашэньня тыповай задачы.</t>
   </si>
 </sst>
 </file>
@@ -290,8 +335,8 @@
   </sheetPr>
   <dimension ref="A1:E733"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -362,11 +407,76 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="52.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>2022032001</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>2022032002</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>2022032003</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="35.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>2022032004</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="51.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <v>2022032005</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Regeneration of files after dictionary update.
</commit_message>
<xml_diff>
--- a/src/main/resources/Слоўнік Пугачова.xlsx
+++ b/src/main/resources/Слоўнік Пугачова.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
   <si>
     <t xml:space="preserve">BFD</t>
   </si>
@@ -170,6 +170,15 @@
   </si>
   <si>
     <t xml:space="preserve">звычайна выкарыстоўваецца для выкананьня нейкай аперацыі, патрэбнай у дадзены момант. Найбольш распаўсюджана ў кантэксце правядзеньня плацяжоў, таму для такіх выпадкаў можа мець месца больш разгорнуты пераклад - аднаразовая спасылка для аплаты.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vCard, VCF, Virtual Contact File</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vCard, VCF, віртуальны файл кантакту, электронная візітоўка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">стандарт для фармату файла электроннай візітоўкі. vCard можа быць прымацавана да ліста, дасланага з электроннац пошты, MMS ці QR-кода. Можа зьмяшчаць у сабе імя, адкрас, нумар тэлефону, электронную пошту й г.д.</t>
   </si>
 </sst>
 </file>
@@ -420,15 +429,15 @@
   <dimension ref="A1:E733"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="28.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="45.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="62.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="62.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="29.44"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="2" width="14.43"/>
@@ -673,7 +682,20 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="74.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="n">
+        <v>2022032902</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Regeneration of files after converter update. Added new term.
</commit_message>
<xml_diff>
--- a/src/main/resources/Слоўнік Пугачова.xlsx
+++ b/src/main/resources/Слоўнік Пугачова.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="68">
   <si>
     <t xml:space="preserve">BFD</t>
   </si>
@@ -160,11 +160,11 @@
     <t xml:space="preserve">Шматфактарная аўтэнтыфікацыя</t>
   </si>
   <si>
-    <t xml:space="preserve">працэс праверкі таго, што карыстальнік зьяўляецца тым, за каго сябе выдае праз больш чым адзін фактар. 
+    <t xml:space="preserve">працэс праверкі таго, што карыстальнік зьяўляецца тым, за каго сябе выдае праз больш чым адзін фактар.
 Асноўныя групы фактараў:
 1) Нешта, што чалавек ведае (пароль, асабістая даныя й г.д.)
 2) Нешта, што чалавек мае (іншы акаўнт, прылада й г.д.)
-3) Нешта, што зьяўляецца часткай чалавека (адбітак пальца, скан сетчаткі глаза й г.д.)</t>
+3) Нешта, што зьяўляецца часткай чалавека (адбітак пальца, скан сятчаткі вока й г.д.)</t>
   </si>
   <si>
     <t xml:space="preserve">nonce</t>
@@ -201,7 +201,7 @@
     <t xml:space="preserve">партнёрская спасылка</t>
   </si>
   <si>
-    <t xml:space="preserve">спецыяльны від спасылкі, якую адзін карыстальнік можа даслаць іншаму чалавеку для рэгістрацыі ў пэўнай праграме/сістэме, а пасьля, як правіла, атрымаць бонусы за рэгістрацыю па сваёй спасылцы.</t>
+    <t xml:space="preserve">спэцыяльны від спасылкі, якую адзін карыстальнік можа даслаць іншаму чалавеку для рэгістрацыі ў пэўнай праграме/сыстэме, а пасьля, як правіла, атрымаць бонусы за рэгістрацыю па сваёй спасылцы.</t>
   </si>
   <si>
     <t xml:space="preserve">referral program</t>
@@ -220,6 +220,16 @@
   </si>
   <si>
     <t xml:space="preserve">спецыяльны від спасылкі, якую адзін карыстальнік можа даслаць іншаму чалавеку для рэгістрацыі ў пэўнай, як правіла недаступнай для шырокага кола, праграме/сістэме. У адрозьненьне ад партнёрскай спасылкі бонусы за запрошаных людзей не налічваюцца. Можа мець месца адказнасьць за непрымальныя паводзіны запрошаных карыстальнікаў.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">transaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">трансакцыя</t>
+  </si>
+  <si>
+    <t xml:space="preserve">набор дзеяньняў, якія або выконваюцца ўсе разам, або не выконваецца ні адно зь іх.
+Прыклад: перавод грошай з аднаго рахунка ў адной валюце на другі ў другой. Пасьпяховае выкананьне складаецца з сьпісаньня грошай зь першага рахунка, канвэртацыі й залічэньня на другі рахунак. Сцэнар пры якім грошы сьпішуцца з першага рахунка, а пасьля з-за памылкі яны ня будуць сканвэртаваны й залічаны на другі зьяўляецца недапушчальным. У выпадку памылкі падчас трансакцыі стан аб'ектаў трансакцыі не зьмяняецца.</t>
   </si>
 </sst>
 </file>
@@ -469,8 +479,8 @@
   </sheetPr>
   <dimension ref="A1:E733"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -793,7 +803,20 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="121.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="n">
+        <v>2022050701</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Regeneration of files after converter update.
</commit_message>
<xml_diff>
--- a/src/main/resources/Слоўнік Пугачова.xlsx
+++ b/src/main/resources/Слоўнік Пугачова.xlsx
@@ -28,7 +28,7 @@
     <t xml:space="preserve">Бібліятэка дэскрыптараў бінарных файлаў, ДБФ (The Binary File Descriptor library)</t>
   </si>
   <si>
-    <t xml:space="preserve">асноўны механізм праекта GNU для працы з аб'ектнымі файламі розных фарматаў.</t>
+    <t xml:space="preserve">асноўны мэханізм праекта GNU для працы з аб'ектнымі файламі розных фарматаў.</t>
   </si>
   <si>
     <t xml:space="preserve">relocation</t>
@@ -37,7 +37,7 @@
     <t xml:space="preserve">прысваеньне адрасу</t>
   </si>
   <si>
-    <t xml:space="preserve">працэс прысваеньня адрасоў загрузкі для кода й дадзеных праграмы, якія залежаць ад пазіцыі, і карэкціроўкі кода й даных для адлюстраваньня прысвоеных адрасоў. </t>
+    <t xml:space="preserve">працэс прысваеньня адрасоў загрузкі для кода й дадзеных праграмы, якія залежаць ад пазыцыі, і карэкціроўкі кода й даных для адлюстраваньня прысвоеных адрасоў.</t>
   </si>
   <si>
     <t xml:space="preserve">Layout features</t>
@@ -46,7 +46,7 @@
     <t xml:space="preserve">Інструмэнты разьметкі</t>
   </si>
   <si>
-    <t xml:space="preserve">уключаюць у сябе тлусты тэкст, падкрэсліваньне, розныя шрыфты й вялікія/загалоўныя літары. Тыповыя інструмэнты разьметкі залежаць ад тыпу тэксту. Вялікія тэксты звычайна разбіваюцца на раздзелы, каб спрасьціць успрыманьне інфармацыі. </t>
+    <t xml:space="preserve">уключаюць у сябе тлусты тэкст, падкрэсьліваньне, розныя шрыфты й вялікія/загалоўныя літары. Тыповыя інструмэнты разьметкі залежаць ад тыпу тэксту. Вялікія тэксты звычайна разьбіваюцца на разьдзелы, каб спрасьціць успрыманьне інфармацыі.</t>
   </si>
   <si>
     <t xml:space="preserve">Variation Axes</t>
@@ -55,7 +55,7 @@
     <t xml:space="preserve">Восі варыяцый</t>
   </si>
   <si>
-    <t xml:space="preserve">дыяпазон лікаў для значэньня, якое апісвае вызначаны аспект дызайну канкрэтнага элемента.</t>
+    <t xml:space="preserve">дыяпазон лікаў для значэньня, якое апісвае вызначаны аспэкт дызайну канкрэтнага элемэнта.</t>
   </si>
   <si>
     <t xml:space="preserve">CJK Symbols and Punctuation</t>
@@ -70,10 +70,10 @@
     <t xml:space="preserve">mkmk, Mark to Mark Positioning</t>
   </si>
   <si>
-    <t xml:space="preserve">Пазіцыяванне акцэнтаў адносна акцэнтаў</t>
-  </si>
-  <si>
-    <t xml:space="preserve">асаблівасьць OpenType, якая дазваляе пазіцыянаваць акцэнты адносна іншых акцэнтаў</t>
+    <t xml:space="preserve">Пазыцыяванне акцэнтаў адносна акцэнтаў</t>
+  </si>
+  <si>
+    <t xml:space="preserve">асаблівасьць OpenType, якая дазваляе пазыцыянаваць акцэнты адносна іншых акцэнтаў</t>
   </si>
   <si>
     <t xml:space="preserve">Reverse engineering</t>
@@ -91,7 +91,7 @@
     <t xml:space="preserve">Аб'ектна-арыентаванае праграміраваньне</t>
   </si>
   <si>
-    <t xml:space="preserve">падыход да напісаньня коду, пры якім сістэма апісваецца праз аб'екты і іх узаемадзеяньне. Метады й палі з інфармацыяй у гэтым выпадку ня могуць існаваць па-за аб'ектам.</t>
+    <t xml:space="preserve">падыход да напісаньня коду, пры якім сыстэма апісваецца праз аб'екты і іх узаемадзеяньне. Мэтады й палі з інфармацыяй у гэтым выпадку ня могуць існаваць па-за абʼектам.</t>
   </si>
   <si>
     <t xml:space="preserve">Software design pattern</t>
@@ -124,7 +124,7 @@
     <t xml:space="preserve">Аўтэнтыфкацыя з дапамогай ключоў SSH</t>
   </si>
   <si>
-    <t xml:space="preserve">больш бяспечная альтэрнатыва клясычнай аўтэнтыфікацыі праз імя й пароль з выкарыстаньнем ключоў SSH. На сэрверы разьмяшчаецца адкрыты ключ, з дапамогай якога зашыфроўваецца паведамленьне й дасылаецца кліенту. Кліент з дапамогай закрытага ключа можа расшыфраваць паведамленьне й даслаць сэрверу адказ. У гэтай схеме галоўнае каб ніхто не завалодаў закрытым ключом кліента, інакш ён зможа прайсьці аўтэнтыфікацыю замест яго.</t>
+    <t xml:space="preserve">больш бясьпечная альтэрнатыва клясычнай аўтэнтыфікацыі праз імя й пароль з выкарыстаньнем ключоў SSH. На сэрвэры разьмяшчаецца адкрыты ключ, з дапамогай якога зашыфроўваецца паведамленьне й дасылаецца кліенту. Кліент з дапамогай закрытага ключа можа расшыфраваць паведамленьне й даслаць сэрвэру адказ. У гэтай схеме галоўнае каб ніхто не завалодаў закрытым ключом кліента, інакш ён зможа прайсьці аўтэнтыфікацыю замест яго.</t>
   </si>
   <si>
     <t xml:space="preserve">Identification</t>
@@ -151,7 +151,7 @@
     <t xml:space="preserve">Аўтарызацыя</t>
   </si>
   <si>
-    <t xml:space="preserve">працэс прадстаўленьня карыстальніку пэўных правоў у сістэме. Для некаторых сістэм неабходна прайсьці аўтэнтыфікацыю для атрыманьня правоў. Некаторыя сістэмы дазваляюць любым карыстальнікам выконваць пэўныя дзеяньні (то бок без аўтэнтыфікацыі).</t>
+    <t xml:space="preserve">працэс прадстаўленьня карыстальніку пэўных правоў у сыстэме. Для некаторых сыстэм неабходна прайсьці аўтэнтыфікацыю для атрыманьня правоў. Некаторыя сыстэмы дазваляюць любым карыстальнікам выконваць пэўныя дзеяньні (то бок без аўтэнтыфікацыі).</t>
   </si>
   <si>
     <t xml:space="preserve">Multi-Factor Authentication (MFA)</t>
@@ -182,7 +182,7 @@
     <t xml:space="preserve">vCard, VCF, віртуальны файл кантакту, электронная візітоўка</t>
   </si>
   <si>
-    <t xml:space="preserve">стандарт для фармату файла электроннай візітоўкі. vCard можа быць прымацавана да ліста, дасланага з электроннай пошты, MMS ці QR-кода. Можа зьмяшчаць у сабе імя, адрас, нумар тэлефону й г.д.</t>
+    <t xml:space="preserve">стандарт для фармату файла электроннай візытоўкі. vCard можа быць прымацавана да ліста, дасланага з электроннай пошты, MMS ці QR-кода. Можа зьмяшчаць у сабе імя, адрас, нумар тэлефону й г.д.</t>
   </si>
   <si>
     <t xml:space="preserve">revoke session</t>
@@ -191,8 +191,7 @@
     <t xml:space="preserve">скончыць сесію</t>
   </si>
   <si>
-    <t xml:space="preserve">правесьці адмену аўтарызацыі карыстальніка. Можна зрабіць для прылады, зь якой непасрэдна ўзаемадзейнічае карыстальнік, або для аддаленых прылад.
-Для перакладаў сустракаюцца варыянты «закончыць сесію» або «закрыць сесію». Варыянт «адклікаць сесію» зьяўляецца сумнеўным.</t>
+    <t xml:space="preserve">правесьці адмену аўтарызацыі карыстальніка. Можна зрабіць для прылады, зь якой непасрэдна ўзаемадзейнічае карыстальнік, або для аддаленых прылад.</t>
   </si>
   <si>
     <t xml:space="preserve">referral link</t>
@@ -219,7 +218,7 @@
     <t xml:space="preserve">запрашальная спасылка</t>
   </si>
   <si>
-    <t xml:space="preserve">спецыяльны від спасылкі, якую адзін карыстальнік можа даслаць іншаму чалавеку для рэгістрацыі ў пэўнай, як правіла недаступнай для шырокага кола, праграме/сістэме. У адрозьненьне ад партнёрскай спасылкі бонусы за запрошаных людзей не налічваюцца. Можа мець месца адказнасьць за непрымальныя паводзіны запрошаных карыстальнікаў.</t>
+    <t xml:space="preserve">спэцыяльны від спасылкі, якую адзін карыстальнік можа даслаць іншаму чалавеку для рэгістрацыі ў пэўнай, як правіла недаступнай для шырокага кола, праграме/сыстэме. У адрозьненьне ад партнэрскай спасылкі бонусы за запрошаных людзей не налічваюцца. Можа мець месца адказнасьць за непрымальныя паводзіны запрошаных карыстальнікаў.</t>
   </si>
   <si>
     <t xml:space="preserve">transaction</t>
@@ -479,8 +478,8 @@
   </sheetPr>
   <dimension ref="A1:E733"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>